<commit_message>
knn model, best k value algorithm, figure out why it's overfitting on accuracy_score
</commit_message>
<xml_diff>
--- a/predictions.xlsx
+++ b/predictions.xlsx
@@ -1161,7 +1161,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -1476,7 +1476,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -2646,7 +2646,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -3231,7 +3231,7 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4446,7 +4446,7 @@
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4491,7 +4491,7 @@
       </c>
       <c r="K90" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4716,7 +4716,7 @@
       </c>
       <c r="K95" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4941,7 +4941,7 @@
       </c>
       <c r="K100" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -4986,7 +4986,7 @@
       </c>
       <c r="K101" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5031,7 +5031,7 @@
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5121,7 +5121,7 @@
       </c>
       <c r="K104" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5211,7 +5211,7 @@
       </c>
       <c r="K106" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5481,7 +5481,7 @@
       </c>
       <c r="K112" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5796,7 +5796,7 @@
       </c>
       <c r="K119" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5886,7 +5886,7 @@
       </c>
       <c r="K121" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6246,7 +6246,7 @@
       </c>
       <c r="K129" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6516,7 +6516,7 @@
       </c>
       <c r="K135" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6921,7 +6921,7 @@
       </c>
       <c r="K144" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7911,7 +7911,7 @@
       </c>
       <c r="K166" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8226,7 +8226,7 @@
       </c>
       <c r="K173" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8271,7 +8271,7 @@
       </c>
       <c r="K174" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8406,7 +8406,7 @@
       </c>
       <c r="K177" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8496,7 +8496,7 @@
       </c>
       <c r="K179" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8631,7 +8631,7 @@
       </c>
       <c r="K182" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -8721,7 +8721,7 @@
       </c>
       <c r="K184" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -9531,7 +9531,7 @@
       </c>
       <c r="K202" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -10071,7 +10071,7 @@
       </c>
       <c r="K214" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -10296,7 +10296,7 @@
       </c>
       <c r="K219" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -10566,7 +10566,7 @@
       </c>
       <c r="K225" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -10746,7 +10746,7 @@
       </c>
       <c r="K229" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -10971,7 +10971,7 @@
       </c>
       <c r="K234" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12591,7 +12591,7 @@
       </c>
       <c r="K270" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12681,7 +12681,7 @@
       </c>
       <c r="K272" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -12816,7 +12816,7 @@
       </c>
       <c r="K275" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -13221,7 +13221,7 @@
       </c>
       <c r="K284" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -13491,7 +13491,7 @@
       </c>
       <c r="K290" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -13716,7 +13716,7 @@
       </c>
       <c r="K295" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14301,7 +14301,7 @@
       </c>
       <c r="K308" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14436,7 +14436,7 @@
       </c>
       <c r="K311" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14616,7 +14616,7 @@
       </c>
       <c r="K315" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -14976,7 +14976,7 @@
       </c>
       <c r="K323" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15246,7 +15246,7 @@
       </c>
       <c r="K329" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15381,7 +15381,7 @@
       </c>
       <c r="K332" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15561,7 +15561,7 @@
       </c>
       <c r="K336" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15651,7 +15651,7 @@
       </c>
       <c r="K338" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16236,7 +16236,7 @@
       </c>
       <c r="K351" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16776,7 +16776,7 @@
       </c>
       <c r="K363" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17136,7 +17136,7 @@
       </c>
       <c r="K371" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17406,7 +17406,7 @@
       </c>
       <c r="K377" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17586,7 +17586,7 @@
       </c>
       <c r="K381" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17721,7 +17721,7 @@
       </c>
       <c r="K384" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -18261,7 +18261,7 @@
       </c>
       <c r="K396" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -18666,7 +18666,7 @@
       </c>
       <c r="K405" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -18936,7 +18936,7 @@
       </c>
       <c r="K411" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19026,7 +19026,7 @@
       </c>
       <c r="K413" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19296,7 +19296,7 @@
       </c>
       <c r="K419" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -19791,7 +19791,7 @@
       </c>
       <c r="K430" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -20196,7 +20196,7 @@
       </c>
       <c r="K439" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -20601,7 +20601,7 @@
       </c>
       <c r="K448" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -20736,7 +20736,7 @@
       </c>
       <c r="K451" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21051,7 +21051,7 @@
       </c>
       <c r="K458" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21501,7 +21501,7 @@
       </c>
       <c r="K468" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21996,7 +21996,7 @@
       </c>
       <c r="K479" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23346,7 +23346,7 @@
       </c>
       <c r="K509" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23481,7 +23481,7 @@
       </c>
       <c r="K512" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23526,7 +23526,7 @@
       </c>
       <c r="K513" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23751,7 +23751,7 @@
       </c>
       <c r="K518" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -23886,7 +23886,7 @@
       </c>
       <c r="K521" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -24021,7 +24021,7 @@
       </c>
       <c r="K524" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -24156,7 +24156,7 @@
       </c>
       <c r="K527" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -24246,7 +24246,7 @@
       </c>
       <c r="K529" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -24291,7 +24291,7 @@
       </c>
       <c r="K530" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -24696,7 +24696,7 @@
       </c>
       <c r="K539" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -25146,7 +25146,7 @@
       </c>
       <c r="K549" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -25191,7 +25191,7 @@
       </c>
       <c r="K550" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -25236,7 +25236,7 @@
       </c>
       <c r="K551" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -25326,7 +25326,7 @@
       </c>
       <c r="K553" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -25821,7 +25821,7 @@
       </c>
       <c r="K564" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -25911,7 +25911,7 @@
       </c>
       <c r="K566" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -26001,7 +26001,7 @@
       </c>
       <c r="K568" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -26046,7 +26046,7 @@
       </c>
       <c r="K569" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -26091,7 +26091,7 @@
       </c>
       <c r="K570" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -26136,7 +26136,7 @@
       </c>
       <c r="K571" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -26406,7 +26406,7 @@
       </c>
       <c r="K577" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -26451,7 +26451,7 @@
       </c>
       <c r="K578" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -26946,7 +26946,7 @@
       </c>
       <c r="K589" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -27036,7 +27036,7 @@
       </c>
       <c r="K591" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -28611,7 +28611,7 @@
       </c>
       <c r="K626" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -28701,7 +28701,7 @@
       </c>
       <c r="K628" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -29601,7 +29601,7 @@
       </c>
       <c r="K648" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -29781,7 +29781,7 @@
       </c>
       <c r="K652" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -30051,7 +30051,7 @@
       </c>
       <c r="K658" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -30096,7 +30096,7 @@
       </c>
       <c r="K659" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -30951,7 +30951,7 @@
       </c>
       <c r="K678" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -30996,7 +30996,7 @@
       </c>
       <c r="K679" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -31761,7 +31761,7 @@
       </c>
       <c r="K696" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -31806,7 +31806,7 @@
       </c>
       <c r="K697" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -31851,7 +31851,7 @@
       </c>
       <c r="K698" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -32121,7 +32121,7 @@
       </c>
       <c r="K704" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -32436,7 +32436,7 @@
       </c>
       <c r="K711" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -33111,7 +33111,7 @@
       </c>
       <c r="K726" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -33156,7 +33156,7 @@
       </c>
       <c r="K727" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -33201,7 +33201,7 @@
       </c>
       <c r="K728" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -33696,7 +33696,7 @@
       </c>
       <c r="K739" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -33741,7 +33741,7 @@
       </c>
       <c r="K740" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -35451,7 +35451,7 @@
       </c>
       <c r="K778" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -36171,7 +36171,7 @@
       </c>
       <c r="K794" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -36891,7 +36891,7 @@
       </c>
       <c r="K810" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -37161,7 +37161,7 @@
       </c>
       <c r="K816" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -37476,7 +37476,7 @@
       </c>
       <c r="K823" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -37611,7 +37611,7 @@
       </c>
       <c r="K826" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -37926,7 +37926,7 @@
       </c>
       <c r="K833" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -38196,7 +38196,7 @@
       </c>
       <c r="K839" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -38241,7 +38241,7 @@
       </c>
       <c r="K840" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -38691,7 +38691,7 @@
       </c>
       <c r="K850" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -38826,7 +38826,7 @@
       </c>
       <c r="K853" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -39006,7 +39006,7 @@
       </c>
       <c r="K857" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -39906,7 +39906,7 @@
       </c>
       <c r="K877" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -40131,7 +40131,7 @@
       </c>
       <c r="K882" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -40626,7 +40626,7 @@
       </c>
       <c r="K893" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -40941,7 +40941,7 @@
       </c>
       <c r="K900" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -41796,7 +41796,7 @@
       </c>
       <c r="K919" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -41841,7 +41841,7 @@
       </c>
       <c r="K920" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -43821,7 +43821,7 @@
       </c>
       <c r="K964" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -44316,7 +44316,7 @@
       </c>
       <c r="K975" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -44586,7 +44586,7 @@
       </c>
       <c r="K981" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -44676,7 +44676,7 @@
       </c>
       <c r="K983" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -44991,7 +44991,7 @@
       </c>
       <c r="K990" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Standardization, starting from k = 2 to prevent overfitting, added plotting
</commit_message>
<xml_diff>
--- a/predictions.xlsx
+++ b/predictions.xlsx
@@ -1026,7 +1026,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -1656,7 +1656,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -1746,7 +1746,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -1791,7 +1791,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -1836,7 +1836,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -1926,7 +1926,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -2196,7 +2196,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -2736,7 +2736,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -3411,7 +3411,7 @@
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -3501,7 +3501,7 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -3771,7 +3771,7 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -4446,7 +4446,7 @@
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -4491,7 +4491,7 @@
       </c>
       <c r="K90" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -4716,7 +4716,7 @@
       </c>
       <c r="K95" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -4896,7 +4896,7 @@
       </c>
       <c r="K99" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -4986,7 +4986,7 @@
       </c>
       <c r="K101" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -5121,7 +5121,7 @@
       </c>
       <c r="K104" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -5211,7 +5211,7 @@
       </c>
       <c r="K106" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -5256,7 +5256,7 @@
       </c>
       <c r="K107" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -5526,7 +5526,7 @@
       </c>
       <c r="K113" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -5796,7 +5796,7 @@
       </c>
       <c r="K119" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -6021,7 +6021,7 @@
       </c>
       <c r="K124" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -6111,7 +6111,7 @@
       </c>
       <c r="K126" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -6246,7 +6246,7 @@
       </c>
       <c r="K129" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -6966,7 +6966,7 @@
       </c>
       <c r="K145" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -7911,7 +7911,7 @@
       </c>
       <c r="K166" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -7956,7 +7956,7 @@
       </c>
       <c r="K167" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -8136,7 +8136,7 @@
       </c>
       <c r="K171" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -8226,7 +8226,7 @@
       </c>
       <c r="K173" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -8271,7 +8271,7 @@
       </c>
       <c r="K174" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -8631,7 +8631,7 @@
       </c>
       <c r="K182" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -9351,7 +9351,7 @@
       </c>
       <c r="K198" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -9441,7 +9441,7 @@
       </c>
       <c r="K200" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -9576,7 +9576,7 @@
       </c>
       <c r="K203" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -9666,7 +9666,7 @@
       </c>
       <c r="K205" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -10161,7 +10161,7 @@
       </c>
       <c r="K216" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -10251,7 +10251,7 @@
       </c>
       <c r="K218" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -10566,7 +10566,7 @@
       </c>
       <c r="K225" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -10701,7 +10701,7 @@
       </c>
       <c r="K228" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -10971,7 +10971,7 @@
       </c>
       <c r="K234" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -11331,7 +11331,7 @@
       </c>
       <c r="K242" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -11691,7 +11691,7 @@
       </c>
       <c r="K250" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -11916,7 +11916,7 @@
       </c>
       <c r="K255" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -12051,7 +12051,7 @@
       </c>
       <c r="K258" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -12231,7 +12231,7 @@
       </c>
       <c r="K262" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -12546,7 +12546,7 @@
       </c>
       <c r="K269" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -12591,7 +12591,7 @@
       </c>
       <c r="K270" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -12681,7 +12681,7 @@
       </c>
       <c r="K272" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -12816,7 +12816,7 @@
       </c>
       <c r="K275" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -12861,7 +12861,7 @@
       </c>
       <c r="K276" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -12996,7 +12996,7 @@
       </c>
       <c r="K279" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -13221,7 +13221,7 @@
       </c>
       <c r="K284" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -13266,7 +13266,7 @@
       </c>
       <c r="K285" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -13401,7 +13401,7 @@
       </c>
       <c r="K288" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -13491,7 +13491,7 @@
       </c>
       <c r="K290" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -13716,7 +13716,7 @@
       </c>
       <c r="K295" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -14121,7 +14121,7 @@
       </c>
       <c r="K304" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -14436,7 +14436,7 @@
       </c>
       <c r="K311" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -14571,7 +14571,7 @@
       </c>
       <c r="K314" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -14706,7 +14706,7 @@
       </c>
       <c r="K317" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -14976,7 +14976,7 @@
       </c>
       <c r="K323" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -15381,7 +15381,7 @@
       </c>
       <c r="K332" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -15471,7 +15471,7 @@
       </c>
       <c r="K334" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -15561,7 +15561,7 @@
       </c>
       <c r="K336" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -15651,7 +15651,7 @@
       </c>
       <c r="K338" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -15876,7 +15876,7 @@
       </c>
       <c r="K343" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -15966,7 +15966,7 @@
       </c>
       <c r="K345" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16011,7 +16011,7 @@
       </c>
       <c r="K346" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16146,7 +16146,7 @@
       </c>
       <c r="K349" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -16236,7 +16236,7 @@
       </c>
       <c r="K351" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -16551,7 +16551,7 @@
       </c>
       <c r="K358" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -16596,7 +16596,7 @@
       </c>
       <c r="K359" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -16776,7 +16776,7 @@
       </c>
       <c r="K363" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -16821,7 +16821,7 @@
       </c>
       <c r="K364" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -16866,7 +16866,7 @@
       </c>
       <c r="K365" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -17046,7 +17046,7 @@
       </c>
       <c r="K369" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -17136,7 +17136,7 @@
       </c>
       <c r="K371" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -17181,7 +17181,7 @@
       </c>
       <c r="K372" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17361,7 +17361,7 @@
       </c>
       <c r="K376" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -17406,7 +17406,7 @@
       </c>
       <c r="K377" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -17676,7 +17676,7 @@
       </c>
       <c r="K383" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -17766,7 +17766,7 @@
       </c>
       <c r="K385" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17856,7 +17856,7 @@
       </c>
       <c r="K387" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -17901,7 +17901,7 @@
       </c>
       <c r="K388" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -18081,7 +18081,7 @@
       </c>
       <c r="K392" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -18261,7 +18261,7 @@
       </c>
       <c r="K396" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -18441,7 +18441,7 @@
       </c>
       <c r="K400" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -18621,7 +18621,7 @@
       </c>
       <c r="K404" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -18666,7 +18666,7 @@
       </c>
       <c r="K405" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -18936,7 +18936,7 @@
       </c>
       <c r="K411" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -19026,7 +19026,7 @@
       </c>
       <c r="K413" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -19161,7 +19161,7 @@
       </c>
       <c r="K416" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -19251,7 +19251,7 @@
       </c>
       <c r="K418" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -19296,7 +19296,7 @@
       </c>
       <c r="K419" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -19701,7 +19701,7 @@
       </c>
       <c r="K428" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -19791,7 +19791,7 @@
       </c>
       <c r="K430" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -20511,7 +20511,7 @@
       </c>
       <c r="K446" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -20601,7 +20601,7 @@
       </c>
       <c r="K448" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -20961,7 +20961,7 @@
       </c>
       <c r="K456" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -21006,7 +21006,7 @@
       </c>
       <c r="K457" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -21051,7 +21051,7 @@
       </c>
       <c r="K458" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -21231,7 +21231,7 @@
       </c>
       <c r="K462" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -21816,7 +21816,7 @@
       </c>
       <c r="K475" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -21906,7 +21906,7 @@
       </c>
       <c r="K477" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -21996,7 +21996,7 @@
       </c>
       <c r="K479" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -22041,7 +22041,7 @@
       </c>
       <c r="K480" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -22131,7 +22131,7 @@
       </c>
       <c r="K482" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -23031,7 +23031,7 @@
       </c>
       <c r="K502" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -23346,7 +23346,7 @@
       </c>
       <c r="K509" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -23526,7 +23526,7 @@
       </c>
       <c r="K513" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -23886,7 +23886,7 @@
       </c>
       <c r="K521" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -23976,7 +23976,7 @@
       </c>
       <c r="K523" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -24021,7 +24021,7 @@
       </c>
       <c r="K524" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -24291,7 +24291,7 @@
       </c>
       <c r="K530" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -24516,7 +24516,7 @@
       </c>
       <c r="K535" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -24921,7 +24921,7 @@
       </c>
       <c r="K544" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -24966,7 +24966,7 @@
       </c>
       <c r="K545" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -25011,7 +25011,7 @@
       </c>
       <c r="K546" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -25146,7 +25146,7 @@
       </c>
       <c r="K549" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -25191,7 +25191,7 @@
       </c>
       <c r="K550" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -25236,7 +25236,7 @@
       </c>
       <c r="K551" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -25416,7 +25416,7 @@
       </c>
       <c r="K555" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -25596,7 +25596,7 @@
       </c>
       <c r="K559" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -25686,7 +25686,7 @@
       </c>
       <c r="K561" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -25731,7 +25731,7 @@
       </c>
       <c r="K562" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -26001,7 +26001,7 @@
       </c>
       <c r="K568" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -26046,7 +26046,7 @@
       </c>
       <c r="K569" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -26091,7 +26091,7 @@
       </c>
       <c r="K570" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -26451,7 +26451,7 @@
       </c>
       <c r="K578" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -26991,7 +26991,7 @@
       </c>
       <c r="K590" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -27036,7 +27036,7 @@
       </c>
       <c r="K591" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -27306,7 +27306,7 @@
       </c>
       <c r="K597" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -27621,7 +27621,7 @@
       </c>
       <c r="K604" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -27801,7 +27801,7 @@
       </c>
       <c r="K608" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -28026,7 +28026,7 @@
       </c>
       <c r="K613" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -28341,7 +28341,7 @@
       </c>
       <c r="K620" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -28431,7 +28431,7 @@
       </c>
       <c r="K622" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -28611,7 +28611,7 @@
       </c>
       <c r="K626" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -28656,7 +28656,7 @@
       </c>
       <c r="K627" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -28701,7 +28701,7 @@
       </c>
       <c r="K628" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -28971,7 +28971,7 @@
       </c>
       <c r="K634" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -29061,7 +29061,7 @@
       </c>
       <c r="K636" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -29196,7 +29196,7 @@
       </c>
       <c r="K639" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -29421,7 +29421,7 @@
       </c>
       <c r="K644" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -29556,7 +29556,7 @@
       </c>
       <c r="K647" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -29601,7 +29601,7 @@
       </c>
       <c r="K648" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -29781,7 +29781,7 @@
       </c>
       <c r="K652" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -29871,7 +29871,7 @@
       </c>
       <c r="K654" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -30096,7 +30096,7 @@
       </c>
       <c r="K659" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -30501,7 +30501,7 @@
       </c>
       <c r="K668" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -30816,7 +30816,7 @@
       </c>
       <c r="K675" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -31131,7 +31131,7 @@
       </c>
       <c r="K682" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -31311,7 +31311,7 @@
       </c>
       <c r="K686" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -31491,7 +31491,7 @@
       </c>
       <c r="K690" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -31581,7 +31581,7 @@
       </c>
       <c r="K692" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -31761,7 +31761,7 @@
       </c>
       <c r="K696" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -31851,7 +31851,7 @@
       </c>
       <c r="K698" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -32121,7 +32121,7 @@
       </c>
       <c r="K704" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -32436,7 +32436,7 @@
       </c>
       <c r="K711" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -32661,7 +32661,7 @@
       </c>
       <c r="K716" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -32976,7 +32976,7 @@
       </c>
       <c r="K723" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -33111,7 +33111,7 @@
       </c>
       <c r="K726" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -33201,7 +33201,7 @@
       </c>
       <c r="K728" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -33426,7 +33426,7 @@
       </c>
       <c r="K733" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -34281,7 +34281,7 @@
       </c>
       <c r="K752" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -34686,7 +34686,7 @@
       </c>
       <c r="K761" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -34911,7 +34911,7 @@
       </c>
       <c r="K766" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -35091,7 +35091,7 @@
       </c>
       <c r="K770" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -35316,7 +35316,7 @@
       </c>
       <c r="K775" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -35496,7 +35496,7 @@
       </c>
       <c r="K779" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -35586,7 +35586,7 @@
       </c>
       <c r="K781" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -35811,7 +35811,7 @@
       </c>
       <c r="K786" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -35856,7 +35856,7 @@
       </c>
       <c r="K787" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -36171,7 +36171,7 @@
       </c>
       <c r="K794" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -36576,7 +36576,7 @@
       </c>
       <c r="K803" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -36891,7 +36891,7 @@
       </c>
       <c r="K810" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -37206,7 +37206,7 @@
       </c>
       <c r="K817" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -37341,7 +37341,7 @@
       </c>
       <c r="K820" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -37476,7 +37476,7 @@
       </c>
       <c r="K823" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -37611,7 +37611,7 @@
       </c>
       <c r="K826" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -37836,7 +37836,7 @@
       </c>
       <c r="K831" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -37926,7 +37926,7 @@
       </c>
       <c r="K833" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -38061,7 +38061,7 @@
       </c>
       <c r="K836" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -38241,7 +38241,7 @@
       </c>
       <c r="K840" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -38286,7 +38286,7 @@
       </c>
       <c r="K841" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -38421,7 +38421,7 @@
       </c>
       <c r="K844" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -38556,7 +38556,7 @@
       </c>
       <c r="K847" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -38691,7 +38691,7 @@
       </c>
       <c r="K850" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -38826,7 +38826,7 @@
       </c>
       <c r="K853" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -38916,7 +38916,7 @@
       </c>
       <c r="K855" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -39141,7 +39141,7 @@
       </c>
       <c r="K860" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -39996,7 +39996,7 @@
       </c>
       <c r="K879" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -40131,7 +40131,7 @@
       </c>
       <c r="K882" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -40311,7 +40311,7 @@
       </c>
       <c r="K886" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -40446,7 +40446,7 @@
       </c>
       <c r="K889" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -40491,7 +40491,7 @@
       </c>
       <c r="K890" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -40626,7 +40626,7 @@
       </c>
       <c r="K893" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -40941,7 +40941,7 @@
       </c>
       <c r="K900" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -41211,7 +41211,7 @@
       </c>
       <c r="K906" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -41706,7 +41706,7 @@
       </c>
       <c r="K917" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -41796,7 +41796,7 @@
       </c>
       <c r="K919" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -41841,7 +41841,7 @@
       </c>
       <c r="K920" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -42201,7 +42201,7 @@
       </c>
       <c r="K928" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -42696,7 +42696,7 @@
       </c>
       <c r="K939" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -42921,7 +42921,7 @@
       </c>
       <c r="K944" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -43101,7 +43101,7 @@
       </c>
       <c r="K948" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -43191,7 +43191,7 @@
       </c>
       <c r="K950" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -43326,7 +43326,7 @@
       </c>
       <c r="K953" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -43371,7 +43371,7 @@
       </c>
       <c r="K954" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -43416,7 +43416,7 @@
       </c>
       <c r="K955" t="inlineStr">
         <is>
-          <t>yes</t>
+          <t>no</t>
         </is>
       </c>
     </row>
@@ -43641,7 +43641,7 @@
       </c>
       <c r="K960" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -44001,7 +44001,7 @@
       </c>
       <c r="K968" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -44136,7 +44136,7 @@
       </c>
       <c r="K971" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -44766,7 +44766,7 @@
       </c>
       <c r="K985" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -44991,7 +44991,7 @@
       </c>
       <c r="K990" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>
@@ -45171,7 +45171,7 @@
       </c>
       <c r="K994" t="inlineStr">
         <is>
-          <t>no</t>
+          <t>yes</t>
         </is>
       </c>
     </row>

</xml_diff>